<commit_message>
AP: Problemas ao crypto_excel
</commit_message>
<xml_diff>
--- a/python-email/dados/dados.xlsx
+++ b/python-email/dados/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Desktop\Automation-Python\python-email\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B5C9C6-1A8F-44F5-A069-172DD25E6CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187DD164-D353-44A6-925F-D9A2E315CF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1695" windowWidth="16200" windowHeight="9360" xr2:uid="{546421D2-C81E-4DCD-B4C3-B8B57E72DF37}"/>
+    <workbookView xWindow="24060" yWindow="1425" windowWidth="16200" windowHeight="9360" xr2:uid="{546421D2-C81E-4DCD-B4C3-B8B57E72DF37}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>OPA</t>
   </si>
   <si>
-    <t>teste,eu,sou,o,jonas,silva;teste;teste;aeeeo;acabouaqui</t>
+    <t>teste,eu,sou,o,jonas,silva;teste;teste;aeeeo;acabouaqui;acaba</t>
   </si>
 </sst>
 </file>

</xml_diff>